<commit_message>
tạo giao diện và update một số file vào csdl
</commit_message>
<xml_diff>
--- a/Design document/can_bo_lop.xlsx
+++ b/Design document/can_bo_lop.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Design document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="198"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -155,32 +159,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -218,331 +203,561 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col min="1" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>14020062</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>34704</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2">
         <v>14020791</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="5">
         <v>35290</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>14020783</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="5">
         <v>35345</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="2">
         <v>14020198</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>35347</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="6">
         <v>14020553</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="5">
         <v>35282</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="2">
         <v>14020581</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="5">
         <v>35137</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="2">
         <v>14020108</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="5">
         <v>35104</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="2">
         <v>14020171</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="5">
         <v>35096</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -551,401 +766,400 @@
       <c r="C10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="11">
         <v>35332</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="9" t="n">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
         <v>14020042</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D11" s="11">
         <v>35120</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="9">
         <v>14020577</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="11" t="n">
+      <c r="D12" s="11">
         <v>35421</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="9">
         <v>14020056</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="11">
         <v>35069</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="2">
         <v>14020002</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="12" t="n">
+      <c r="D14" s="12">
         <v>35321</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="2">
         <v>14020003</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="12" t="n">
+      <c r="D15" s="12">
         <v>35126</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="2">
         <v>14020005</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="12" t="n">
+      <c r="D16" s="12">
         <v>34746</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="2">
         <v>14020652</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="12" t="n">
+      <c r="D17" s="12">
         <v>35176</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="n">
+      <c r="B18" s="13">
         <v>14020655</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="14">
         <v>35413</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="n">
+      <c r="B19" s="13">
         <v>14020065</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="14">
         <v>35348</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="n">
+      <c r="B20" s="13">
         <v>14020103</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="14">
         <v>35394</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="n">
+      <c r="B21" s="13">
         <v>14020113</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="14" t="n">
+      <c r="D21" s="14">
         <v>34717</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="n">
+      <c r="B22" s="15">
         <v>14020071</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="16">
         <v>35271</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="n">
+      <c r="B23" s="15">
         <v>14020080</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="16" t="n">
+      <c r="D23" s="16">
         <v>35373</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="n">
+      <c r="B24" s="15">
         <v>14020657</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="16" t="n">
+      <c r="D24" s="16">
         <v>35145</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="n">
+      <c r="B25" s="15">
         <v>14020117</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="16" t="n">
+      <c r="D25" s="16">
         <v>32470</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="n">
+      <c r="B26" s="15">
         <v>14020041</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="16" t="n">
+      <c r="D26" s="16">
         <v>35325</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="n">
+      <c r="B27" s="15">
         <v>14020580</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="16" t="n">
+      <c r="D27" s="16">
         <v>35359</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="n">
+      <c r="B28" s="15">
         <v>14020076</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="16" t="n">
+      <c r="D28" s="16">
         <v>35308</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="15" t="n">
+      <c r="B29" s="15">
         <v>14020083</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="16" t="n">
+      <c r="D29" s="16">
         <v>35222</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>